<commit_message>
add config for redis mysql
</commit_message>
<xml_diff>
--- a/Lab_Redis/app/Uploads/data.xlsx
+++ b/Lab_Redis/app/Uploads/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6990"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="1" r:id="rId1"/>
     <sheet name="Host" sheetId="2" r:id="rId2"/>
     <sheet name="Virtualization" sheetId="3" r:id="rId3"/>
-    <sheet name="Falcon 404 IP assignment" sheetId="4" r:id="rId4"/>
+    <sheet name="Vlan 404 IP assignment" sheetId="4" r:id="rId4"/>
     <sheet name="Sanblaze" sheetId="5" r:id="rId5"/>
     <sheet name="Rockies" sheetId="6" r:id="rId6"/>
     <sheet name="Service" sheetId="7" r:id="rId7"/>
@@ -32,7 +32,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
     <comment ref="A41" authorId="0">
@@ -45,7 +45,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="693">
   <si>
     <t>Name</t>
   </si>
@@ -615,7 +615,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -633,7 +633,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -654,7 +654,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -675,7 +675,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -696,7 +696,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -729,7 +729,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1809,7 +1809,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1821,7 +1821,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1846,7 +1846,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1857,7 +1857,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2339,7 +2339,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2349,7 +2349,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2369,7 +2369,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2390,7 +2390,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2409,7 +2409,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2423,7 +2423,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2433,7 +2433,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3135,19 +3135,37 @@
   <si>
     <t>10.109.110.92</t>
   </si>
+  <si>
+    <t>10.245.93.48</t>
+  </si>
+  <si>
+    <t>10.245.93.49</t>
+  </si>
+  <si>
+    <t>10.245.93.50</t>
+  </si>
+  <si>
+    <t>10.245.93.51</t>
+  </si>
+  <si>
+    <t>10.245.93.52</t>
+  </si>
+  <si>
+    <t>10.245.93.53</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="176" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3162,21 +3180,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3191,7 +3209,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3225,7 +3243,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3243,7 +3261,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3269,7 +3287,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3300,7 +3318,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3308,7 +3326,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3847,10 +3865,10 @@
     <xf numFmtId="0" fontId="20" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="21" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="21" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4015,9 +4033,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -4047,7 +4065,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4121,7 +4139,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4156,7 +4173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4332,21 +4348,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5346,21 +5362,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.25" customWidth="1"/>
     <col min="7" max="7" width="74" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5410,7 +5426,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.5">
+    <row r="3" spans="1:7" ht="378">
       <c r="A3" s="61" t="s">
         <v>463</v>
       </c>
@@ -5433,7 +5449,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="210">
+    <row r="4" spans="1:7" ht="189">
       <c r="A4" s="61" t="s">
         <v>464</v>
       </c>
@@ -5467,17 +5483,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="55.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1">
@@ -5491,7 +5507,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="69" t="s">
         <v>487</v>
       </c>
@@ -5502,7 +5518,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.75">
+    <row r="3" spans="1:3" ht="24">
       <c r="A3" s="71" t="s">
         <v>490</v>
       </c>
@@ -5656,7 +5672,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="153">
+    <row r="17" spans="1:3" ht="140.25">
       <c r="A17" s="75" t="s">
         <v>515</v>
       </c>
@@ -5806,7 +5822,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="242.25">
+    <row r="31" spans="1:3" ht="229.5">
       <c r="A31" s="75" t="s">
         <v>545</v>
       </c>
@@ -5839,7 +5855,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="36.75">
+    <row r="34" spans="1:3" ht="36">
       <c r="A34" s="75" t="s">
         <v>551</v>
       </c>
@@ -6081,7 +6097,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" ht="14.25">
       <c r="A56" s="84" t="s">
         <v>588</v>
       </c>
@@ -6092,14 +6108,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" ht="14.25">
       <c r="A57" s="84" t="s">
         <v>589</v>
       </c>
       <c r="B57" s="93"/>
       <c r="C57" s="93"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" ht="14.25">
       <c r="A58" s="84" t="s">
         <v>590</v>
       </c>
@@ -6110,7 +6126,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" ht="14.25">
       <c r="A59" s="84" t="s">
         <v>591</v>
       </c>
@@ -6121,14 +6137,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" ht="14.25">
       <c r="A60" s="84" t="s">
         <v>592</v>
       </c>
       <c r="B60" s="97"/>
       <c r="C60" s="97"/>
     </row>
-    <row r="61" spans="1:3" ht="24.75">
+    <row r="61" spans="1:3" ht="14.25">
       <c r="A61" s="84" t="s">
         <v>593</v>
       </c>
@@ -6261,23 +6277,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30">
@@ -6543,23 +6561,24 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6588,7 +6607,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="27">
       <c r="A3" s="121" t="s">
         <v>119</v>
       </c>
@@ -6602,7 +6621,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="40.5">
       <c r="A4" s="121" t="s">
         <v>667</v>
       </c>
@@ -6616,7 +6635,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="27">
       <c r="A5" s="121" t="s">
         <v>668</v>
       </c>
@@ -6631,24 +6650,26 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H98"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:H104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7145,7 +7166,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="15">
       <c r="A23" s="48" t="s">
         <v>380</v>
       </c>
@@ -7167,7 +7188,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="48" t="s">
         <v>380</v>
       </c>
@@ -7189,7 +7210,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="48" t="s">
         <v>380</v>
       </c>
@@ -7211,7 +7232,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="48" t="s">
         <v>380</v>
       </c>
@@ -7233,7 +7254,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="48" t="s">
         <v>380</v>
       </c>
@@ -7255,7 +7276,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="48" t="s">
         <v>380</v>
       </c>
@@ -7277,7 +7298,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="48" t="s">
         <v>380</v>
       </c>
@@ -7301,7 +7322,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="48" t="s">
         <v>380</v>
       </c>
@@ -7369,7 +7390,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="48" t="s">
         <v>380</v>
       </c>
@@ -7391,7 +7412,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="48" t="s">
         <v>380</v>
       </c>
@@ -7413,7 +7434,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="48" t="s">
         <v>380</v>
       </c>
@@ -7437,7 +7458,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="48" t="s">
         <v>380</v>
       </c>
@@ -7459,7 +7480,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="48" t="s">
         <v>380</v>
       </c>
@@ -7481,7 +7502,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="15">
       <c r="A38" s="48" t="s">
         <v>380</v>
       </c>
@@ -7503,7 +7524,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="15">
       <c r="A39" s="48" t="s">
         <v>429</v>
       </c>
@@ -7525,7 +7546,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="15">
       <c r="A40" s="48" t="s">
         <v>380</v>
       </c>
@@ -7547,7 +7568,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="15">
       <c r="A41" s="48" t="s">
         <v>380</v>
       </c>
@@ -7569,7 +7590,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="48" t="s">
         <v>380</v>
       </c>
@@ -7591,7 +7612,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="15">
       <c r="A43" s="48" t="s">
         <v>380</v>
       </c>
@@ -7613,7 +7634,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" ht="15">
       <c r="A44" s="48" t="s">
         <v>380</v>
       </c>
@@ -7635,7 +7656,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" ht="15">
       <c r="A45" s="48" t="s">
         <v>380</v>
       </c>
@@ -8746,6 +8767,126 @@
         <v>17</v>
       </c>
       <c r="H98" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>633</v>
+      </c>
+      <c r="B99" t="s">
+        <v>629</v>
+      </c>
+      <c r="C99" t="s">
+        <v>687</v>
+      </c>
+      <c r="D99" t="s">
+        <v>631</v>
+      </c>
+      <c r="E99" t="s">
+        <v>17</v>
+      </c>
+      <c r="H99" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>633</v>
+      </c>
+      <c r="B100" t="s">
+        <v>629</v>
+      </c>
+      <c r="C100" t="s">
+        <v>688</v>
+      </c>
+      <c r="D100" t="s">
+        <v>631</v>
+      </c>
+      <c r="E100" t="s">
+        <v>17</v>
+      </c>
+      <c r="H100" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>633</v>
+      </c>
+      <c r="B101" t="s">
+        <v>629</v>
+      </c>
+      <c r="C101" t="s">
+        <v>689</v>
+      </c>
+      <c r="D101" t="s">
+        <v>631</v>
+      </c>
+      <c r="E101" t="s">
+        <v>17</v>
+      </c>
+      <c r="H101" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>633</v>
+      </c>
+      <c r="B102" t="s">
+        <v>629</v>
+      </c>
+      <c r="C102" t="s">
+        <v>690</v>
+      </c>
+      <c r="D102" t="s">
+        <v>631</v>
+      </c>
+      <c r="E102" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>633</v>
+      </c>
+      <c r="B103" t="s">
+        <v>629</v>
+      </c>
+      <c r="C103" t="s">
+        <v>691</v>
+      </c>
+      <c r="D103" t="s">
+        <v>631</v>
+      </c>
+      <c r="E103" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="114" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>633</v>
+      </c>
+      <c r="B104" t="s">
+        <v>629</v>
+      </c>
+      <c r="C104" t="s">
+        <v>692</v>
+      </c>
+      <c r="D104" t="s">
+        <v>631</v>
+      </c>
+      <c r="E104" t="s">
+        <v>17</v>
+      </c>
+      <c r="H104" s="114" t="s">
         <v>660</v>
       </c>
     </row>
@@ -8756,20 +8897,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
@@ -9165,21 +9306,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9205,7 +9346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="54">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -9228,7 +9369,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="54">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9251,7 +9392,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="27">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -9455,22 +9596,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
@@ -9634,8 +9775,8 @@
   <conditionalFormatting sqref="E1:F1">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF638EC6"/>
       </dataBar>
       <extLst>
@@ -9669,14 +9810,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
@@ -9797,19 +9938,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -9826,7 +9967,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60">
+    <row r="2" spans="1:4" ht="54">
       <c r="A2" s="31" t="s">
         <v>676</v>
       </c>
@@ -9840,7 +9981,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="105">
+    <row r="3" spans="1:4" ht="94.5">
       <c r="A3" s="31" t="s">
         <v>238</v>
       </c>
@@ -9866,7 +10007,7 @@
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="54">
       <c r="A5" s="31" t="s">
         <v>243</v>
       </c>
@@ -9880,7 +10021,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.25">
       <c r="A6" s="31" t="s">
         <v>246</v>
       </c>
@@ -9963,19 +10104,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="134.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10097,22 +10238,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="14.25">
       <c r="A1" s="42" t="s">
         <v>182</v>
       </c>
@@ -10126,7 +10267,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="42" t="s">
         <v>32</v>
       </c>
@@ -10140,7 +10281,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="14.25">
       <c r="A3" s="42" t="s">
         <v>71</v>
       </c>
@@ -10154,7 +10295,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="14.25">
       <c r="A4" s="42" t="s">
         <v>75</v>
       </c>
@@ -10168,7 +10309,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="14.25">
       <c r="A5" s="42" t="s">
         <v>24</v>
       </c>
@@ -10180,7 +10321,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.25">
       <c r="A6" s="42" t="s">
         <v>18</v>
       </c>
@@ -10192,7 +10333,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="14.25">
       <c r="A7" s="42" t="s">
         <v>23</v>
       </c>
@@ -10204,7 +10345,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="14.25">
       <c r="A8" s="42" t="s">
         <v>79</v>
       </c>
@@ -10218,7 +10359,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="14.25">
       <c r="A9" s="42" t="s">
         <v>36</v>
       </c>
@@ -10230,7 +10371,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="14.25">
       <c r="A10" s="42" t="s">
         <v>42</v>
       </c>
@@ -10242,7 +10383,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="14.25">
       <c r="A11" s="42" t="s">
         <v>47</v>
       </c>
@@ -10254,7 +10395,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="14.25">
       <c r="A12" s="42" t="s">
         <v>52</v>
       </c>
@@ -10266,7 +10407,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="14.25">
       <c r="A13" s="42" t="s">
         <v>57</v>
       </c>
@@ -10280,7 +10421,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="14.25">
       <c r="A14" s="42" t="s">
         <v>61</v>
       </c>
@@ -10292,7 +10433,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="14.25">
       <c r="A15" s="42" t="s">
         <v>65</v>
       </c>
@@ -10304,7 +10445,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="14.25">
       <c r="A16" s="42" t="s">
         <v>70</v>
       </c>

</xml_diff>